<commit_message>
update testcase and danger log
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/Documents/Spring24/ECE568/hw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B5FD0-5E36-7A47-ADBC-2B1995CCFBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8CC0FB-4439-3242-B104-4E0197DC59F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3940" yWindow="760" windowWidth="24800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Extra note to TA</t>
   </si>
@@ -96,7 +96,10 @@
     <t>cache size = 20, LRU policy</t>
   </si>
   <si>
-    <t>The proxy can be run as daemon on VM, and can be run as nornal program on docker, but cannot be run as daemon on docker.</t>
+    <t>The proxy can be run as daemon on VM, and can be run as normal program on docker, but cannot be run as daemon on docker.</t>
+  </si>
+  <si>
+    <t>We use mutex to lock the write operation on cache and log file.</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -159,9 +162,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +488,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -508,6 +516,7 @@
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -516,6 +525,7 @@
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="16" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -524,6 +534,7 @@
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="16" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -532,6 +543,7 @@
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -540,6 +552,7 @@
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" ht="16" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -548,6 +561,7 @@
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="16" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -556,6 +570,7 @@
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -564,7 +579,7 @@
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -575,6 +590,7 @@
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" ht="16" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -583,6 +599,7 @@
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="55" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -591,6 +608,9 @@
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="16" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -599,6 +619,7 @@
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" ht="16" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -607,6 +628,7 @@
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" ht="43" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -615,6 +637,7 @@
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" ht="31" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -623,6 +646,7 @@
       <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" ht="34" customHeight="1">
       <c r="A17" s="1" t="s">
@@ -631,7 +655,7 @@
       <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>